<commit_message>
unification of three versions
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -169,21 +169,21 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="9.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>1</v>
       </c>

</xml_diff>